<commit_message>
rename timetable finish *Einleitung Kryptographie* genaurere Aufteilung in Grundlagen Kryptographie finish *DES, 3DES*
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
   <si>
     <t>Montag</t>
   </si>
@@ -94,13 +94,73 @@
   </si>
   <si>
     <t>Task</t>
+  </si>
+  <si>
+    <t>Programm Validierung</t>
+  </si>
+  <si>
+    <t>Frei</t>
+  </si>
+  <si>
+    <t>Programmierung</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>ABGABE</t>
+  </si>
+  <si>
+    <t>Abschluss</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>FREI / Auswärts</t>
+  </si>
+  <si>
+    <t>Grundlagen Thesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmierung </t>
+  </si>
+  <si>
+    <t>Projektabschluss</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
+  </si>
+  <si>
+    <t>Zeitplan</t>
+  </si>
+  <si>
+    <t>Aufagbe</t>
+  </si>
+  <si>
+    <t>ZUSAMMENFASSUNG</t>
+  </si>
+  <si>
+    <t>heute - 30.07.</t>
+  </si>
+  <si>
+    <t>31.07. - 09.08.</t>
+  </si>
+  <si>
+    <t>10.08. - 30.08.</t>
+  </si>
+  <si>
+    <t>31.08. - 06.09.</t>
+  </si>
+  <si>
+    <t>06.09. - 09.09.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +179,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -165,6 +233,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -466,17 +542,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,6 +580,9 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -514,6 +594,9 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -523,7 +606,10 @@
         <v>41837</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,7 +620,7 @@
         <v>41838</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,7 +653,7 @@
         <v>41841</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,6 +754,593 @@
       <c r="C17" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>41851</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>41852</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3">
+        <v>41853</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3">
+        <v>41854</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3">
+        <v>41855</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>41856</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3">
+        <v>41857</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>41858</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>41859</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="3">
+        <v>41860</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="3">
+        <v>41861</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3">
+        <v>41862</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <v>41863</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="3">
+        <v>41864</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="3">
+        <v>41865</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="3">
+        <v>41866</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="3">
+        <v>41867</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3">
+        <v>41868</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="3">
+        <v>41869</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
+        <v>41870</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3">
+        <v>41871</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3">
+        <v>41872</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="3">
+        <v>41873</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="3">
+        <v>41874</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3">
+        <v>41875</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="3">
+        <v>41876</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3">
+        <v>41877</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3">
+        <v>41878</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="3">
+        <v>41879</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="3">
+        <v>41880</v>
+      </c>
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <v>41881</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="3">
+        <v>41882</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="3">
+        <v>41883</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="3">
+        <v>41884</v>
+      </c>
+      <c r="C51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3">
+        <v>41885</v>
+      </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="3">
+        <v>41886</v>
+      </c>
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="3">
+        <v>41887</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="3">
+        <v>41888</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="3">
+        <v>41889</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="3">
+        <v>41890</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="3">
+        <v>41891</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="3">
+        <v>41892</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>41892</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish *blowfish* delete *PBE*
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="46">
   <si>
     <t>Montag</t>
   </si>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,6 +636,9 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -671,6 +674,9 @@
       </c>
       <c r="C9" t="s">
         <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish *RSA* finish *Betriebsmodi (ECB, CBC, OFB, OCB, CTR)
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="46">
   <si>
     <t>Montag</t>
   </si>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,6 +649,9 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish validation TODO : import graphic, complete TEXT update timetable
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8250"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="46">
   <si>
     <t>Montag</t>
   </si>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -791,7 +791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -801,8 +801,11 @@
       <c r="C18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -812,8 +815,11 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -823,8 +829,11 @@
       <c r="C20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -834,8 +843,11 @@
       <c r="C21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -845,8 +857,11 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -856,8 +871,11 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -867,8 +885,11 @@
       <c r="C24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -878,8 +899,11 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -889,8 +913,11 @@
       <c r="C26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -900,8 +927,11 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -911,8 +941,11 @@
       <c r="C28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -922,8 +955,11 @@
       <c r="C29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -933,8 +969,11 @@
       <c r="C30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -944,8 +983,11 @@
       <c r="C31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -955,8 +997,11 @@
       <c r="C32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -966,8 +1011,11 @@
       <c r="C33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -977,8 +1025,11 @@
       <c r="C34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -988,8 +1039,11 @@
       <c r="C35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -999,8 +1053,11 @@
       <c r="C36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1010,8 +1067,11 @@
       <c r="C37" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1021,8 +1081,11 @@
       <c r="C38" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1032,8 +1095,11 @@
       <c r="C39" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1043,8 +1109,11 @@
       <c r="C40" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1054,8 +1123,11 @@
       <c r="C41" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1065,8 +1137,11 @@
       <c r="C42" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1076,8 +1151,11 @@
       <c r="C43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1087,8 +1165,11 @@
       <c r="C44" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1098,8 +1179,11 @@
       <c r="C45" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1109,8 +1193,11 @@
       <c r="C46" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>5</v>
       </c>

</xml_diff>